<commit_message>
comments from amr and ahmed
</commit_message>
<xml_diff>
--- a/.eventra/Progress Review + Design Studio + KPIs Roadmap.xlsx
+++ b/.eventra/Progress Review + Design Studio + KPIs Roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marketing Manager\Desktop\Agent X\EVENTRA X\Eventra Code V1.1\eventra\.eventra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E1573B-5E60-4186-B45C-00F0B63F53D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92851BA6-E4F5-416A-BCA1-92C1BA61B2F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C7039EC2-77ED-45F3-AE04-C9B46F5B5812}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="385">
   <si>
     <t>Category</t>
   </si>
@@ -969,6 +969,234 @@
   </si>
   <si>
     <t>Community</t>
+  </si>
+  <si>
+    <t>Date Validation</t>
+  </si>
+  <si>
+    <t>Event start and end date can be a previous date. End date can be before the start date.</t>
+  </si>
+  <si>
+    <t>Exhibitors</t>
+  </si>
+  <si>
+    <t>Frontend Related</t>
+  </si>
+  <si>
+    <t>Add/Edit button not working or slow; multiple clicks add multiple exhibitors. View does not redirect back to exhibitor page after adding. Same issues (email, phone, image, filter/sort) as Speakers.</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>State Management</t>
+  </si>
+  <si>
+    <t>Going to another tab or refreshing reloads the website and loses unsaved information. Current state should be preserved.</t>
+  </si>
+  <si>
+    <t>Attendees</t>
+  </si>
+  <si>
+    <t>Error 'failing to add attendee' shown even though attendee is added successfully.</t>
+  </si>
+  <si>
+    <t>Creating more than one session in the same room/time shows error but needs a clearer notification for the user.</t>
+  </si>
+  <si>
+    <t>Logic</t>
+  </si>
+  <si>
+    <t>Live preview registration link: needs implementation of attendees table, check if Eventra user (Boolean), and B2B redirection flow logic.</t>
+  </si>
+  <si>
+    <t>Forms</t>
+  </si>
+  <si>
+    <t>Need implementation for form links, form_id/type storage, and results dashboard. No 'Choose Template' option currently available.</t>
+  </si>
+  <si>
+    <t>Browse Events</t>
+  </si>
+  <si>
+    <t>Visibility</t>
+  </si>
+  <si>
+    <t>Events created do not show in 'Browse Events' tab when signed out.</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Dummy user email (user@example.com) is showing when browsing events.</t>
+  </si>
+  <si>
+    <t>B2B</t>
+  </si>
+  <si>
+    <t>Need mechanism for attendees/exhibitors to book B2B discussions (notify manager or direct link).</t>
+  </si>
+  <si>
+    <t>Sign Up</t>
+  </si>
+  <si>
+    <t>Country code selector in Phone Number input is tilted/misaligned.</t>
+  </si>
+  <si>
+    <t>Filters</t>
+  </si>
+  <si>
+    <t>'Choose Date Range' filter is not functional.</t>
+  </si>
+  <si>
+    <t>Choosing both 'Free' and 'Paid' filters results in no events showing.</t>
+  </si>
+  <si>
+    <t>Category filter is not functional and yields no output.</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Search events by date needs clear format (DD-MM-YYYY) or calendar; currently not functional.</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Notifications</t>
+  </si>
+  <si>
+    <t>Notification bell shows red circle even without new notifications. Should only show when unread.</t>
+  </si>
+  <si>
+    <t>User Preferences</t>
+  </si>
+  <si>
+    <t>Liked/Favourite events return to unliked state upon refreshing the page.</t>
+  </si>
+  <si>
+    <t>Two overlapping components observed in Create Event view.</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>User can 'Save &amp; Continue' to skip steps without entering required data (e.g., Step 1 to 2 with 0% completion).</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Paid event option is locked and shows error 'wizard.details.errors.proFeaturePaid'.</t>
+  </si>
+  <si>
+    <t>'Add to maps' button functionality is unclear; behaves exactly like 'View larger map'.</t>
+  </si>
+  <si>
+    <t>Choosing Registration Builder path automatically marks Step 2 as completed and directs to Step 3.</t>
+  </si>
+  <si>
+    <t>Hybrid events should have separate limits and waitlists for in-person vs virtual attendees.</t>
+  </si>
+  <si>
+    <t>Registration Setup</t>
+  </si>
+  <si>
+    <t>'Tickets' option in Step 3 is visible for a second then disappears automatically.</t>
+  </si>
+  <si>
+    <t>Cannot edit or crop uploaded speaker profile image.</t>
+  </si>
+  <si>
+    <t>Adding speaker phone number needs country code selector. Currently defaults to +1 automatically.</t>
+  </si>
+  <si>
+    <t>Selection bar buttons (Export, Send Email, Delete) are not functioning.</t>
+  </si>
+  <si>
+    <t>Creating speaker adds them automatically without option to add timing, location, or capacity.</t>
+  </si>
+  <si>
+    <t>Public Page</t>
+  </si>
+  <si>
+    <t>'Get in touch' button has white text on white background.</t>
+  </si>
+  <si>
+    <t>Search, Filter, and Sort buttons in Speaker Management are not functioning.</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>No email format restriction for speakers or attendees (manual input). Accepts invalid formats.</t>
+  </si>
+  <si>
+    <t>Import CSV issues: Needs file format description, column name strictness. Fails on second attempt. UI doesn't show uploaded list.</t>
+  </si>
+  <si>
+    <t>Export schedule not working. Unknown 3rd export option visible.</t>
+  </si>
+  <si>
+    <t>Changing tabs in Step 3 always resets view to first substep (Speakers) and resets progress percentage.</t>
+  </si>
+  <si>
+    <t>Step count confusion (shows 12, then 11, then 12). Progress bar percentages are inaccurate.</t>
+  </si>
+  <si>
+    <t>Sponsors</t>
+  </si>
+  <si>
+    <t>Send email to sponsor is not functional.</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>UI Suggestion: Place 'Manage Packages' before 'Sponsors' in the layout.</t>
+  </si>
+  <si>
+    <t>Need ability to customize package price for a specific sponsor.</t>
+  </si>
+  <si>
+    <t>Need ability to add or remove specific benefits for a sponsor package.</t>
+  </si>
+  <si>
+    <t>Billing</t>
+  </si>
+  <si>
+    <t>'Upgrade to Pro' leads to static page with no back option; upgrade functionality missing.</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Created marketing links are not visible or copyable.</t>
+  </si>
+  <si>
+    <t>Changing fonts does not apply changes. Edit buttons for side options (About, Details, Agenda) not working.</t>
+  </si>
+  <si>
+    <t>Key Highlights/Takeaways section not working/updating.</t>
+  </si>
+  <si>
+    <t>Settings option for sections (Details, Agenda, Speakers) not working.</t>
+  </si>
+  <si>
+    <t>Full screen mode prevents scrolling and editing; cannot see added sections.</t>
+  </si>
+  <si>
+    <t>Footer hyperlinks not working/navigating.</t>
+  </si>
+  <si>
+    <t>Session can be created with only name, ignoring required fields. Not updating in session list.</t>
+  </si>
+  <si>
+    <t>Preview</t>
+  </si>
+  <si>
+    <t>Preview button not working before publishing event.</t>
   </si>
 </sst>
 </file>
@@ -1044,7 +1272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1063,6 +1291,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1598,10 +1827,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E1D7A6-FA3F-4C2A-A779-5FF7F633A273}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1950,7 +2179,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1970,7 +2199,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>308</v>
       </c>
@@ -1988,6 +2217,1110 @@
       </c>
       <c r="G18" t="s">
         <v>298</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>309</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" t="s">
+        <v>310</v>
+      </c>
+      <c r="I19" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>311</v>
+      </c>
+      <c r="D20" t="s">
+        <v>312</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" t="s">
+        <v>313</v>
+      </c>
+      <c r="I20" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>314</v>
+      </c>
+      <c r="B21" t="s">
+        <v>315</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" t="s">
+        <v>316</v>
+      </c>
+      <c r="I21" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>317</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" t="s">
+        <v>318</v>
+      </c>
+      <c r="I22" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" t="s">
+        <v>319</v>
+      </c>
+      <c r="I23" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>299</v>
+      </c>
+      <c r="B24" t="s">
+        <v>320</v>
+      </c>
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" t="s">
+        <v>321</v>
+      </c>
+      <c r="I24" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>322</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" t="s">
+        <v>323</v>
+      </c>
+      <c r="I25" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>324</v>
+      </c>
+      <c r="B26" t="s">
+        <v>325</v>
+      </c>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" t="s">
+        <v>326</v>
+      </c>
+      <c r="I26" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>324</v>
+      </c>
+      <c r="B27" t="s">
+        <v>327</v>
+      </c>
+      <c r="D27" t="s">
+        <v>312</v>
+      </c>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" t="s">
+        <v>328</v>
+      </c>
+      <c r="I27" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>308</v>
+      </c>
+      <c r="B28" t="s">
+        <v>329</v>
+      </c>
+      <c r="D28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" t="s">
+        <v>330</v>
+      </c>
+      <c r="I28" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>331</v>
+      </c>
+      <c r="D29" t="s">
+        <v>312</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" t="s">
+        <v>332</v>
+      </c>
+      <c r="I29" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>324</v>
+      </c>
+      <c r="B30" t="s">
+        <v>333</v>
+      </c>
+      <c r="D30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" t="s">
+        <v>334</v>
+      </c>
+      <c r="I30" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>324</v>
+      </c>
+      <c r="B31" t="s">
+        <v>333</v>
+      </c>
+      <c r="D31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" t="s">
+        <v>335</v>
+      </c>
+      <c r="I31" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>324</v>
+      </c>
+      <c r="B32" t="s">
+        <v>333</v>
+      </c>
+      <c r="D32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" t="s">
+        <v>336</v>
+      </c>
+      <c r="I32" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>324</v>
+      </c>
+      <c r="B33" t="s">
+        <v>337</v>
+      </c>
+      <c r="D33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" t="s">
+        <v>338</v>
+      </c>
+      <c r="I33" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>339</v>
+      </c>
+      <c r="B34" t="s">
+        <v>340</v>
+      </c>
+      <c r="D34" t="s">
+        <v>312</v>
+      </c>
+      <c r="E34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" t="s">
+        <v>341</v>
+      </c>
+      <c r="I34" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>324</v>
+      </c>
+      <c r="B35" t="s">
+        <v>342</v>
+      </c>
+      <c r="D35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" t="s">
+        <v>343</v>
+      </c>
+      <c r="I35" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>327</v>
+      </c>
+      <c r="D36" t="s">
+        <v>312</v>
+      </c>
+      <c r="E36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" t="s">
+        <v>344</v>
+      </c>
+      <c r="I36" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>345</v>
+      </c>
+      <c r="D37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37" t="s">
+        <v>346</v>
+      </c>
+      <c r="I37" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>347</v>
+      </c>
+      <c r="D38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" t="s">
+        <v>24</v>
+      </c>
+      <c r="G38" t="s">
+        <v>348</v>
+      </c>
+      <c r="I38" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" t="s">
+        <v>312</v>
+      </c>
+      <c r="E39" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" t="s">
+        <v>349</v>
+      </c>
+      <c r="I39" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" t="s">
+        <v>345</v>
+      </c>
+      <c r="D40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" t="s">
+        <v>350</v>
+      </c>
+      <c r="I40" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" t="s">
+        <v>347</v>
+      </c>
+      <c r="D41" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" t="s">
+        <v>351</v>
+      </c>
+      <c r="I41" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" t="s">
+        <v>352</v>
+      </c>
+      <c r="D42" t="s">
+        <v>312</v>
+      </c>
+      <c r="E42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" t="s">
+        <v>24</v>
+      </c>
+      <c r="G42" t="s">
+        <v>353</v>
+      </c>
+      <c r="I42" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="D43" t="s">
+        <v>312</v>
+      </c>
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" t="s">
+        <v>354</v>
+      </c>
+      <c r="I43" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" t="s">
+        <v>41</v>
+      </c>
+      <c r="D44" t="s">
+        <v>312</v>
+      </c>
+      <c r="E44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" t="s">
+        <v>355</v>
+      </c>
+      <c r="I44" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" t="s">
+        <v>41</v>
+      </c>
+      <c r="D45" t="s">
+        <v>312</v>
+      </c>
+      <c r="E45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" t="s">
+        <v>25</v>
+      </c>
+      <c r="G45" t="s">
+        <v>356</v>
+      </c>
+      <c r="I45" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" t="s">
+        <v>357</v>
+      </c>
+      <c r="I46" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>358</v>
+      </c>
+      <c r="B47" t="s">
+        <v>327</v>
+      </c>
+      <c r="D47" t="s">
+        <v>312</v>
+      </c>
+      <c r="E47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" t="s">
+        <v>359</v>
+      </c>
+      <c r="I47" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" t="s">
+        <v>360</v>
+      </c>
+      <c r="I48" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" t="s">
+        <v>361</v>
+      </c>
+      <c r="D49" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" t="s">
+        <v>362</v>
+      </c>
+      <c r="I49" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" t="s">
+        <v>317</v>
+      </c>
+      <c r="D50" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" t="s">
+        <v>24</v>
+      </c>
+      <c r="G50" t="s">
+        <v>363</v>
+      </c>
+      <c r="I50" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" t="s">
+        <v>45</v>
+      </c>
+      <c r="D51" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" t="s">
+        <v>25</v>
+      </c>
+      <c r="G51" t="s">
+        <v>364</v>
+      </c>
+      <c r="I51" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" t="s">
+        <v>345</v>
+      </c>
+      <c r="D52" t="s">
+        <v>312</v>
+      </c>
+      <c r="E52" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" t="s">
+        <v>365</v>
+      </c>
+      <c r="I52" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" t="s">
+        <v>345</v>
+      </c>
+      <c r="D53" t="s">
+        <v>312</v>
+      </c>
+      <c r="E53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" t="s">
+        <v>366</v>
+      </c>
+      <c r="I53" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" t="s">
+        <v>367</v>
+      </c>
+      <c r="D54" t="s">
+        <v>21</v>
+      </c>
+      <c r="E54" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" t="s">
+        <v>368</v>
+      </c>
+      <c r="I54" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" t="s">
+        <v>367</v>
+      </c>
+      <c r="D55" t="s">
+        <v>312</v>
+      </c>
+      <c r="E55" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" t="s">
+        <v>369</v>
+      </c>
+      <c r="G55" t="s">
+        <v>370</v>
+      </c>
+      <c r="I55" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>32</v>
+      </c>
+      <c r="B56" t="s">
+        <v>367</v>
+      </c>
+      <c r="D56" t="s">
+        <v>21</v>
+      </c>
+      <c r="E56" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" t="s">
+        <v>25</v>
+      </c>
+      <c r="G56" t="s">
+        <v>371</v>
+      </c>
+      <c r="I56" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>32</v>
+      </c>
+      <c r="B57" t="s">
+        <v>367</v>
+      </c>
+      <c r="D57" t="s">
+        <v>21</v>
+      </c>
+      <c r="E57" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" t="s">
+        <v>25</v>
+      </c>
+      <c r="G57" t="s">
+        <v>372</v>
+      </c>
+      <c r="I57" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>339</v>
+      </c>
+      <c r="B58" t="s">
+        <v>373</v>
+      </c>
+      <c r="D58" t="s">
+        <v>21</v>
+      </c>
+      <c r="E58" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" t="s">
+        <v>24</v>
+      </c>
+      <c r="G58" t="s">
+        <v>374</v>
+      </c>
+      <c r="I58" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>32</v>
+      </c>
+      <c r="B59" t="s">
+        <v>375</v>
+      </c>
+      <c r="D59" t="s">
+        <v>21</v>
+      </c>
+      <c r="E59" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" t="s">
+        <v>25</v>
+      </c>
+      <c r="G59" t="s">
+        <v>376</v>
+      </c>
+      <c r="I59" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>32</v>
+      </c>
+      <c r="B60" t="s">
+        <v>307</v>
+      </c>
+      <c r="D60" t="s">
+        <v>312</v>
+      </c>
+      <c r="E60" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" t="s">
+        <v>24</v>
+      </c>
+      <c r="G60" t="s">
+        <v>377</v>
+      </c>
+      <c r="I60" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61" t="s">
+        <v>307</v>
+      </c>
+      <c r="D61" t="s">
+        <v>312</v>
+      </c>
+      <c r="E61" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" t="s">
+        <v>25</v>
+      </c>
+      <c r="G61" t="s">
+        <v>378</v>
+      </c>
+      <c r="I61" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62" t="s">
+        <v>307</v>
+      </c>
+      <c r="D62" t="s">
+        <v>312</v>
+      </c>
+      <c r="E62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" t="s">
+        <v>25</v>
+      </c>
+      <c r="G62" t="s">
+        <v>379</v>
+      </c>
+      <c r="I62" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>32</v>
+      </c>
+      <c r="B63" t="s">
+        <v>307</v>
+      </c>
+      <c r="D63" t="s">
+        <v>312</v>
+      </c>
+      <c r="E63" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" t="s">
+        <v>25</v>
+      </c>
+      <c r="G63" t="s">
+        <v>380</v>
+      </c>
+      <c r="I63" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>32</v>
+      </c>
+      <c r="B64" t="s">
+        <v>307</v>
+      </c>
+      <c r="D64" t="s">
+        <v>312</v>
+      </c>
+      <c r="E64" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" t="s">
+        <v>25</v>
+      </c>
+      <c r="G64" t="s">
+        <v>381</v>
+      </c>
+      <c r="I64" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>32</v>
+      </c>
+      <c r="B65" t="s">
+        <v>45</v>
+      </c>
+      <c r="D65" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" t="s">
+        <v>25</v>
+      </c>
+      <c r="G65" t="s">
+        <v>382</v>
+      </c>
+      <c r="I65" s="10">
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>32</v>
+      </c>
+      <c r="B66" t="s">
+        <v>383</v>
+      </c>
+      <c r="D66" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" t="s">
+        <v>25</v>
+      </c>
+      <c r="G66" t="s">
+        <v>384</v>
+      </c>
+      <c r="I66" s="10">
+        <v>46047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>